<commit_message>
ajout des cours dans le dossier 4 et début du cours sur sql
</commit_message>
<xml_diff>
--- a/5_Exercices_En_Cours_Formation/6-SQL/1-Exo-MCDMerise/exoTP2_scolaritéEISTI.xlsx
+++ b/5_Exercices_En_Cours_Formation/6-SQL/1-Exo-MCDMerise/exoTP2_scolaritéEISTI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>infirmieres</t>
   </si>
@@ -65,9 +65,6 @@
     <t>année</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>Mnénomique</t>
   </si>
   <si>
@@ -147,6 +144,15 @@
   </si>
   <si>
     <t>id_annee</t>
+  </si>
+  <si>
+    <t>projet</t>
+  </si>
+  <si>
+    <t>epreuve</t>
+  </si>
+  <si>
+    <t>matière</t>
   </si>
 </sst>
 </file>
@@ -613,7 +619,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,13 +647,13 @@
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -658,13 +664,13 @@
         <v>12</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -676,6 +682,9 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
       <c r="L5" s="9"/>
@@ -685,30 +694,33 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
       <c r="J7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -716,13 +728,13 @@
         <v>8</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -730,13 +742,13 @@
         <v>9</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -744,75 +756,75 @@
         <v>5</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J12" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J14" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J15" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J16" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="J17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="9:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J18" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="12"/>

</xml_diff>